<commit_message>
Minor changes with stats code
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/sentiment_indepth.xlsx
+++ b/data_exploration/acl/tables/sentiment_indepth.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>Language</t>
   </si>
@@ -521,7 +521,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +680,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -700,6 +703,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -972,6 +978,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -1018,6 +1027,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -1110,6 +1122,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
       <c r="B25" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Updated sentiment data details
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/sentiment_indepth.xlsx
+++ b/data_exploration/acl/tables/sentiment_indepth.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>Language</t>
   </si>
@@ -521,7 +521,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,6 +594,9 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
       <c r="F3">
         <v>1472</v>
       </c>

</xml_diff>